<commit_message>
compliance bugfixes up through gpt4 dp convo 14
</commit_message>
<xml_diff>
--- a/Data/Creative_Writing_Compliance.xlsx
+++ b/Data/Creative_Writing_Compliance.xlsx
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -499,7 +499,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -512,7 +512,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -642,7 +642,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -694,7 +694,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -733,7 +733,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -746,7 +746,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -759,7 +759,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -772,7 +772,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -850,7 +850,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -876,7 +876,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -980,7 +980,7 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1006,7 +1006,7 @@
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1045,7 +1045,7 @@
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -1071,7 +1071,7 @@
         <v>48</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -1084,7 +1084,7 @@
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -1279,7 +1279,7 @@
         <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -1292,7 +1292,7 @@
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -1318,7 +1318,7 @@
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -1383,7 +1383,7 @@
         <v>72</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -1448,7 +1448,7 @@
         <v>77</v>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -1487,7 +1487,7 @@
         <v>80</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -1539,7 +1539,7 @@
         <v>84</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -1591,7 +1591,7 @@
         <v>88</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -1643,7 +1643,7 @@
         <v>92</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
@@ -1656,7 +1656,7 @@
         <v>93</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -1721,7 +1721,7 @@
         <v>98</v>
       </c>
       <c r="C99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -1877,7 +1877,7 @@
         <v>10</v>
       </c>
       <c r="C111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -1981,7 +1981,7 @@
         <v>18</v>
       </c>
       <c r="C119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -2163,7 +2163,7 @@
         <v>32</v>
       </c>
       <c r="C133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134">
@@ -2202,7 +2202,7 @@
         <v>35</v>
       </c>
       <c r="C136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137">
@@ -2280,7 +2280,7 @@
         <v>41</v>
       </c>
       <c r="C142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
@@ -2345,7 +2345,7 @@
         <v>46</v>
       </c>
       <c r="C147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148">
@@ -2358,7 +2358,7 @@
         <v>47</v>
       </c>
       <c r="C148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
@@ -2371,7 +2371,7 @@
         <v>48</v>
       </c>
       <c r="C149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150">
@@ -2436,7 +2436,7 @@
         <v>53</v>
       </c>
       <c r="C154" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155">
@@ -2501,7 +2501,7 @@
         <v>58</v>
       </c>
       <c r="C159" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160">
@@ -2553,7 +2553,7 @@
         <v>62</v>
       </c>
       <c r="C163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
@@ -2670,7 +2670,7 @@
         <v>71</v>
       </c>
       <c r="C172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173">
@@ -2722,7 +2722,7 @@
         <v>75</v>
       </c>
       <c r="C176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
@@ -2800,7 +2800,7 @@
         <v>81</v>
       </c>
       <c r="C182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183">
@@ -2839,7 +2839,7 @@
         <v>84</v>
       </c>
       <c r="C185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">
@@ -2878,7 +2878,7 @@
         <v>87</v>
       </c>
       <c r="C188" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189">
@@ -2930,7 +2930,7 @@
         <v>91</v>
       </c>
       <c r="C192" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193">
@@ -2943,7 +2943,7 @@
         <v>92</v>
       </c>
       <c r="C193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194">
@@ -3034,7 +3034,7 @@
         <v>99</v>
       </c>
       <c r="C200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201">
@@ -3164,7 +3164,7 @@
         <v>9</v>
       </c>
       <c r="C210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211">
@@ -3177,7 +3177,7 @@
         <v>10</v>
       </c>
       <c r="C211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212">
@@ -3281,7 +3281,7 @@
         <v>18</v>
       </c>
       <c r="C219" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="220">
@@ -3411,7 +3411,7 @@
         <v>28</v>
       </c>
       <c r="C229" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230">
@@ -3554,7 +3554,7 @@
         <v>39</v>
       </c>
       <c r="C240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="241">
@@ -3619,7 +3619,7 @@
         <v>44</v>
       </c>
       <c r="C245" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="246">
@@ -3671,7 +3671,7 @@
         <v>48</v>
       </c>
       <c r="C249" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="250">
@@ -3749,7 +3749,7 @@
         <v>54</v>
       </c>
       <c r="C255" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="256">
@@ -3892,7 +3892,7 @@
         <v>65</v>
       </c>
       <c r="C266" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267">
@@ -3905,7 +3905,7 @@
         <v>66</v>
       </c>
       <c r="C267" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="268">
@@ -3983,7 +3983,7 @@
         <v>72</v>
       </c>
       <c r="C273" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="274">
@@ -4217,7 +4217,7 @@
         <v>90</v>
       </c>
       <c r="C291" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="292">
@@ -4230,7 +4230,7 @@
         <v>91</v>
       </c>
       <c r="C292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="293">
@@ -4438,7 +4438,7 @@
         <v>7</v>
       </c>
       <c r="C308" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="309">
@@ -4451,7 +4451,7 @@
         <v>8</v>
       </c>
       <c r="C309" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="310">
@@ -4841,7 +4841,7 @@
         <v>38</v>
       </c>
       <c r="C339" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="340">
@@ -5049,7 +5049,7 @@
         <v>54</v>
       </c>
       <c r="C355" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="356">
@@ -5205,7 +5205,7 @@
         <v>66</v>
       </c>
       <c r="C367" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="368">
@@ -5218,7 +5218,7 @@
         <v>67</v>
       </c>
       <c r="C368" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="369">
@@ -5361,7 +5361,7 @@
         <v>78</v>
       </c>
       <c r="C379" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="380">
@@ -5465,7 +5465,7 @@
         <v>86</v>
       </c>
       <c r="C387" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="388">
@@ -5699,7 +5699,7 @@
         <v>4</v>
       </c>
       <c r="C405" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="406">
@@ -5738,7 +5738,7 @@
         <v>7</v>
       </c>
       <c r="C408" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="409">
@@ -6037,7 +6037,7 @@
         <v>30</v>
       </c>
       <c r="C431" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="432">
@@ -6219,7 +6219,7 @@
         <v>44</v>
       </c>
       <c r="C445" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="446">
@@ -6375,7 +6375,7 @@
         <v>56</v>
       </c>
       <c r="C457" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="458">
@@ -6505,7 +6505,7 @@
         <v>66</v>
       </c>
       <c r="C467" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="468">
@@ -6518,7 +6518,7 @@
         <v>67</v>
       </c>
       <c r="C468" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="469">
@@ -6570,7 +6570,7 @@
         <v>71</v>
       </c>
       <c r="C472" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="473">
@@ -6687,7 +6687,7 @@
         <v>80</v>
       </c>
       <c r="C481" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="482">
@@ -6778,7 +6778,7 @@
         <v>87</v>
       </c>
       <c r="C488" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="489">
@@ -6804,7 +6804,7 @@
         <v>89</v>
       </c>
       <c r="C490" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="491">
@@ -6999,7 +6999,7 @@
         <v>4</v>
       </c>
       <c r="C505" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="506">
@@ -7181,7 +7181,7 @@
         <v>18</v>
       </c>
       <c r="C519" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="520">
@@ -7545,7 +7545,7 @@
         <v>46</v>
       </c>
       <c r="C547" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="548">
@@ -7623,7 +7623,7 @@
         <v>52</v>
       </c>
       <c r="C553" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="554">
@@ -7831,7 +7831,7 @@
         <v>68</v>
       </c>
       <c r="C569" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="570">
@@ -8143,7 +8143,7 @@
         <v>92</v>
       </c>
       <c r="C593" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="594">
@@ -8338,7 +8338,7 @@
         <v>7</v>
       </c>
       <c r="C608" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="609">
@@ -9326,7 +9326,7 @@
         <v>83</v>
       </c>
       <c r="C684" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="685">
@@ -9794,7 +9794,7 @@
         <v>19</v>
       </c>
       <c r="C720" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="721">
@@ -9976,7 +9976,7 @@
         <v>33</v>
       </c>
       <c r="C734" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="735">
@@ -10002,7 +10002,7 @@
         <v>35</v>
       </c>
       <c r="C736" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="737">
@@ -10015,7 +10015,7 @@
         <v>36</v>
       </c>
       <c r="C737" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="738">
@@ -10106,7 +10106,7 @@
         <v>43</v>
       </c>
       <c r="C744" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="745">
@@ -10171,7 +10171,7 @@
         <v>48</v>
       </c>
       <c r="C749" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="750">
@@ -10340,7 +10340,7 @@
         <v>61</v>
       </c>
       <c r="C762" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="763">
@@ -10392,7 +10392,7 @@
         <v>65</v>
       </c>
       <c r="C766" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="767">
@@ -10431,7 +10431,7 @@
         <v>68</v>
       </c>
       <c r="C769" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="770">
@@ -10470,7 +10470,7 @@
         <v>71</v>
       </c>
       <c r="C772" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="773">
@@ -10561,7 +10561,7 @@
         <v>78</v>
       </c>
       <c r="C779" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="780">
@@ -10574,7 +10574,7 @@
         <v>79</v>
       </c>
       <c r="C780" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="781">
@@ -10587,7 +10587,7 @@
         <v>80</v>
       </c>
       <c r="C781" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="782">
@@ -10613,7 +10613,7 @@
         <v>82</v>
       </c>
       <c r="C783" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="784">
@@ -10717,7 +10717,7 @@
         <v>90</v>
       </c>
       <c r="C791" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="792">
@@ -10730,7 +10730,7 @@
         <v>91</v>
       </c>
       <c r="C792" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="793">
@@ -10756,7 +10756,7 @@
         <v>93</v>
       </c>
       <c r="C794" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="795">
@@ -10834,7 +10834,7 @@
         <v>99</v>
       </c>
       <c r="C800" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="801">
@@ -10847,7 +10847,7 @@
         <v>100</v>
       </c>
       <c r="C801" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="802">
@@ -10977,7 +10977,7 @@
         <v>10</v>
       </c>
       <c r="C811" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="812">
@@ -11094,7 +11094,7 @@
         <v>19</v>
       </c>
       <c r="C820" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="821">
@@ -11107,7 +11107,7 @@
         <v>20</v>
       </c>
       <c r="C821" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="822">
@@ -11380,7 +11380,7 @@
         <v>41</v>
       </c>
       <c r="C842" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="843">
@@ -11549,7 +11549,7 @@
         <v>54</v>
       </c>
       <c r="C855" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="856">
@@ -11562,7 +11562,7 @@
         <v>55</v>
       </c>
       <c r="C856" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="857">
@@ -11601,7 +11601,7 @@
         <v>58</v>
       </c>
       <c r="C859" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="860">
@@ -11744,7 +11744,7 @@
         <v>69</v>
       </c>
       <c r="C870" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="871">
@@ -11887,7 +11887,7 @@
         <v>80</v>
       </c>
       <c r="C881" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="882">
@@ -12121,7 +12121,7 @@
         <v>98</v>
       </c>
       <c r="C899" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="900">
@@ -12251,7 +12251,7 @@
         <v>8</v>
       </c>
       <c r="C909" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="910">
@@ -12446,7 +12446,7 @@
         <v>23</v>
       </c>
       <c r="C924" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="925">
@@ -12706,7 +12706,7 @@
         <v>43</v>
       </c>
       <c r="C944" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="945">
@@ -12745,7 +12745,7 @@
         <v>46</v>
       </c>
       <c r="C947" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="948">
@@ -12836,7 +12836,7 @@
         <v>53</v>
       </c>
       <c r="C954" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="955">
@@ -12875,7 +12875,7 @@
         <v>56</v>
       </c>
       <c r="C957" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="958">
@@ -12940,7 +12940,7 @@
         <v>61</v>
       </c>
       <c r="C962" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="963">
@@ -12992,7 +12992,7 @@
         <v>65</v>
       </c>
       <c r="C966" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="967">
@@ -13070,7 +13070,7 @@
         <v>71</v>
       </c>
       <c r="C972" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="973">
@@ -13200,7 +13200,7 @@
         <v>81</v>
       </c>
       <c r="C982" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="983">
@@ -13330,7 +13330,7 @@
         <v>91</v>
       </c>
       <c r="C992" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="993">
@@ -13616,7 +13616,7 @@
         <v>13</v>
       </c>
       <c r="C1014" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1015">
@@ -13733,7 +13733,7 @@
         <v>22</v>
       </c>
       <c r="C1023" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1024">
@@ -13785,7 +13785,7 @@
         <v>26</v>
       </c>
       <c r="C1027" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1028">
@@ -13798,7 +13798,7 @@
         <v>27</v>
       </c>
       <c r="C1028" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1029">
@@ -13928,7 +13928,7 @@
         <v>37</v>
       </c>
       <c r="C1038" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1039">
@@ -14071,7 +14071,7 @@
         <v>48</v>
       </c>
       <c r="C1049" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1050">
@@ -14318,7 +14318,7 @@
         <v>67</v>
       </c>
       <c r="C1068" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1069">
@@ -14357,7 +14357,7 @@
         <v>70</v>
       </c>
       <c r="C1071" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1072">
@@ -14708,7 +14708,7 @@
         <v>97</v>
       </c>
       <c r="C1098" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1099">
@@ -14734,7 +14734,7 @@
         <v>99</v>
       </c>
       <c r="C1100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1101">
@@ -14864,7 +14864,7 @@
         <v>9</v>
       </c>
       <c r="C1110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1111">
@@ -14981,7 +14981,7 @@
         <v>18</v>
       </c>
       <c r="C1119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1120">
@@ -15059,7 +15059,7 @@
         <v>24</v>
       </c>
       <c r="C1125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1126">
@@ -15111,7 +15111,7 @@
         <v>28</v>
       </c>
       <c r="C1129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1130">
@@ -15696,7 +15696,7 @@
         <v>73</v>
       </c>
       <c r="C1174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1175">
@@ -16346,7 +16346,7 @@
         <v>23</v>
       </c>
       <c r="C1224" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1225">
@@ -16411,7 +16411,7 @@
         <v>28</v>
       </c>
       <c r="C1229" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1230">
@@ -16437,7 +16437,7 @@
         <v>30</v>
       </c>
       <c r="C1231" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1232">
@@ -16710,7 +16710,7 @@
         <v>51</v>
       </c>
       <c r="C1252" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1253">
@@ -17373,7 +17373,7 @@
         <v>2</v>
       </c>
       <c r="C1303" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1304">
@@ -17607,7 +17607,7 @@
         <v>20</v>
       </c>
       <c r="C1321" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1322">
@@ -17620,7 +17620,7 @@
         <v>21</v>
       </c>
       <c r="C1322" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1323">
@@ -17750,7 +17750,7 @@
         <v>31</v>
       </c>
       <c r="C1332" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1333">
@@ -17893,7 +17893,7 @@
         <v>42</v>
       </c>
       <c r="C1343" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1344">
@@ -17984,7 +17984,7 @@
         <v>49</v>
       </c>
       <c r="C1350" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1351">
@@ -18023,7 +18023,7 @@
         <v>52</v>
       </c>
       <c r="C1353" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1354">
@@ -18140,7 +18140,7 @@
         <v>61</v>
       </c>
       <c r="C1362" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1363">
@@ -18270,7 +18270,7 @@
         <v>71</v>
       </c>
       <c r="C1372" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1373">
@@ -18348,7 +18348,7 @@
         <v>77</v>
       </c>
       <c r="C1378" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1379">
@@ -18361,7 +18361,7 @@
         <v>78</v>
       </c>
       <c r="C1379" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1380">
@@ -18426,7 +18426,7 @@
         <v>83</v>
       </c>
       <c r="C1384" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1385">
@@ -18452,7 +18452,7 @@
         <v>85</v>
       </c>
       <c r="C1386" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1387">
@@ -18647,7 +18647,7 @@
         <v>100</v>
       </c>
       <c r="C1401" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1402">
@@ -18829,7 +18829,7 @@
         <v>14</v>
       </c>
       <c r="C1415" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1416">
@@ -19128,7 +19128,7 @@
         <v>37</v>
       </c>
       <c r="C1438" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1439">
@@ -19583,7 +19583,7 @@
         <v>72</v>
       </c>
       <c r="C1473" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1474">
@@ -19752,7 +19752,7 @@
         <v>85</v>
       </c>
       <c r="C1486" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1487">
@@ -19765,7 +19765,7 @@
         <v>86</v>
       </c>
       <c r="C1487" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1488">
@@ -19778,7 +19778,7 @@
         <v>87</v>
       </c>
       <c r="C1488" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1489">
@@ -19947,7 +19947,7 @@
         <v>100</v>
       </c>
       <c r="C1501" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1502">
@@ -20064,7 +20064,7 @@
         <v>9</v>
       </c>
       <c r="C1510" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1511">
@@ -20116,7 +20116,7 @@
         <v>13</v>
       </c>
       <c r="C1514" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1515">
@@ -20389,7 +20389,7 @@
         <v>34</v>
       </c>
       <c r="C1535" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1536">
@@ -20714,7 +20714,7 @@
         <v>59</v>
       </c>
       <c r="C1560" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1561">
@@ -20792,7 +20792,7 @@
         <v>65</v>
       </c>
       <c r="C1566" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1567">
@@ -21013,7 +21013,7 @@
         <v>82</v>
       </c>
       <c r="C1583" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1584">
@@ -21052,7 +21052,7 @@
         <v>85</v>
       </c>
       <c r="C1586" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1587">
@@ -21130,7 +21130,7 @@
         <v>91</v>
       </c>
       <c r="C1592" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1593">
@@ -21208,7 +21208,7 @@
         <v>97</v>
       </c>
       <c r="C1598" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1599">
@@ -21221,7 +21221,7 @@
         <v>98</v>
       </c>
       <c r="C1599" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1600">

</xml_diff>

<commit_message>
some progress on cw compliance
</commit_message>
<xml_diff>
--- a/Data/Creative_Writing_Compliance.xlsx
+++ b/Data/Creative_Writing_Compliance.xlsx
@@ -11042,7 +11042,7 @@
         <v>15</v>
       </c>
       <c r="C816" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="817">
@@ -11055,7 +11055,7 @@
         <v>16</v>
       </c>
       <c r="C817" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="818">
@@ -11276,7 +11276,7 @@
         <v>33</v>
       </c>
       <c r="C834" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="835">
@@ -11692,7 +11692,7 @@
         <v>65</v>
       </c>
       <c r="C866" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="867">
@@ -11718,7 +11718,7 @@
         <v>67</v>
       </c>
       <c r="C868" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="869">
@@ -12212,7 +12212,7 @@
         <v>5</v>
       </c>
       <c r="C906" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="907">
@@ -12394,7 +12394,7 @@
         <v>19</v>
       </c>
       <c r="C920" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="921">
@@ -12485,7 +12485,7 @@
         <v>26</v>
       </c>
       <c r="C927" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="928">
@@ -12602,7 +12602,7 @@
         <v>35</v>
       </c>
       <c r="C936" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="937">
@@ -13148,7 +13148,7 @@
         <v>77</v>
       </c>
       <c r="C978" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="979">
@@ -13369,7 +13369,7 @@
         <v>94</v>
       </c>
       <c r="C995" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="996">
@@ -13382,7 +13382,7 @@
         <v>95</v>
       </c>
       <c r="C996" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="997">
@@ -13876,7 +13876,7 @@
         <v>33</v>
       </c>
       <c r="C1034" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1035">
@@ -14214,7 +14214,7 @@
         <v>59</v>
       </c>
       <c r="C1060" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1061">
@@ -14474,7 +14474,7 @@
         <v>79</v>
       </c>
       <c r="C1080" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1081">
@@ -14656,7 +14656,7 @@
         <v>93</v>
       </c>
       <c r="C1094" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1095">
@@ -14747,7 +14747,7 @@
         <v>100</v>
       </c>
       <c r="C1101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1102">
@@ -15657,7 +15657,7 @@
         <v>70</v>
       </c>
       <c r="C1171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1172">
@@ -15917,7 +15917,7 @@
         <v>90</v>
       </c>
       <c r="C1191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1192">
@@ -17282,7 +17282,7 @@
         <v>95</v>
       </c>
       <c r="C1296" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1297">
@@ -17321,7 +17321,7 @@
         <v>98</v>
       </c>
       <c r="C1299" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1300">
@@ -18582,7 +18582,7 @@
         <v>95</v>
       </c>
       <c r="C1396" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1397">
@@ -18907,7 +18907,7 @@
         <v>20</v>
       </c>
       <c r="C1421" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1422">
@@ -18933,7 +18933,7 @@
         <v>22</v>
       </c>
       <c r="C1423" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1424">
@@ -18985,7 +18985,7 @@
         <v>26</v>
       </c>
       <c r="C1427" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1428">
@@ -19011,7 +19011,7 @@
         <v>28</v>
       </c>
       <c r="C1429" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1430">
@@ -19557,7 +19557,7 @@
         <v>70</v>
       </c>
       <c r="C1471" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1472">
@@ -19869,7 +19869,7 @@
         <v>94</v>
       </c>
       <c r="C1495" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1496">
@@ -20012,7 +20012,7 @@
         <v>5</v>
       </c>
       <c r="C1506" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1507">
@@ -20831,7 +20831,7 @@
         <v>68</v>
       </c>
       <c r="C1569" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1570">
@@ -21182,7 +21182,7 @@
         <v>95</v>
       </c>
       <c r="C1596" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1597">

</xml_diff>